<commit_message>
Test parsing of xlsx loan registry
</commit_message>
<xml_diff>
--- a/public/templates/loans_template.xlsx
+++ b/public/templates/loans_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/von-christian/Projects/coop_catalyst/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2521F7DF-DF04-FA40-8F4A-F64EACE2BA91}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2FC549B8-D854-054F-9BD1-78698EAA5CA3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16460" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Loan Template</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>Cut-off Date</t>
-  </si>
-  <si>
     <t>Middle Name</t>
   </si>
   <si>
@@ -72,13 +69,37 @@
     <t>Regular Loan</t>
   </si>
   <si>
-    <t>Xhris</t>
-  </si>
-  <si>
     <t>Member</t>
   </si>
   <si>
-    <t>testtig olan</t>
+    <t>Cut Off Date</t>
+  </si>
+  <si>
+    <t>December 31, 2018</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>current_loan</t>
+  </si>
+  <si>
+    <t>October 19, 2018</t>
+  </si>
+  <si>
+    <t>Maturity Date</t>
+  </si>
+  <si>
+    <t>March 19, 2019</t>
+  </si>
+  <si>
+    <t>Pumihic</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Allan Turing</t>
   </si>
 </sst>
 </file>
@@ -115,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -138,11 +159,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -152,6 +184,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -536,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -550,33 +588,34 @@
     <col min="5" max="5" width="15.33203125"/>
     <col min="6" max="6" width="11.5"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="15"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="16.5" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="1028" width="11.5"/>
+    <col min="8" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="15"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="14" max="14" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="1029" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -584,7 +623,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -593,7 +632,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
@@ -601,31 +640,40 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>9</v>
+      <c r="N2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>10000</v>
@@ -633,17 +681,28 @@
       <c r="F3">
         <v>5000</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
       <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="3">
-        <v>43373</v>
+      <c r="O3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>